<commit_message>
feat: Ingredient E number and Ingredient category presentation format options #19
</commit_message>
<xml_diff>
--- a/wwwroot/elabel-ingredients.xlsx
+++ b/wwwroot/elabel-ingredients.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20404"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20407"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\ELabel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\ELabel\wwwroot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30F1A9E7-55F5-41B9-AFF5-1B226D17E50D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C9803E6-FA4D-41EB-9055-DE8C8B7FA490}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13905" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="101">
   <si>
     <t>Id</t>
   </si>
@@ -320,6 +320,9 @@
   </si>
   <si>
     <t>Yeast mannoproteins</t>
+  </si>
+  <si>
+    <t>Enumber</t>
   </si>
 </sst>
 </file>
@@ -680,23 +683,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AC34"/>
+  <dimension ref="A1:AD34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -707,85 +709,88 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -795,17 +800,17 @@
       <c r="C2" t="s">
         <v>31</v>
       </c>
-      <c r="D2" t="b">
-        <v>0</v>
-      </c>
       <c r="E2" t="b">
         <v>0</v>
       </c>
-      <c r="K2" t="s">
+      <c r="F2" t="b">
+        <v>0</v>
+      </c>
+      <c r="L2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -815,17 +820,20 @@
       <c r="C3" t="s">
         <v>34</v>
       </c>
-      <c r="D3" t="b">
-        <v>0</v>
+      <c r="D3">
+        <v>300</v>
       </c>
       <c r="E3" t="b">
         <v>0</v>
       </c>
-      <c r="K3" t="s">
+      <c r="F3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -835,17 +843,17 @@
       <c r="C4" t="s">
         <v>37</v>
       </c>
-      <c r="D4" t="b">
-        <v>0</v>
-      </c>
       <c r="E4" t="b">
         <v>0</v>
       </c>
-      <c r="K4" t="s">
+      <c r="F4" t="b">
+        <v>0</v>
+      </c>
+      <c r="L4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>38</v>
       </c>
@@ -855,17 +863,20 @@
       <c r="C5" t="s">
         <v>31</v>
       </c>
-      <c r="D5" t="b">
-        <v>0</v>
+      <c r="D5">
+        <v>150</v>
       </c>
       <c r="E5" t="b">
         <v>0</v>
       </c>
-      <c r="K5" t="s">
+      <c r="F5" t="b">
+        <v>0</v>
+      </c>
+      <c r="L5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -875,17 +886,20 @@
       <c r="C6" t="s">
         <v>42</v>
       </c>
-      <c r="D6" t="b">
-        <v>0</v>
+      <c r="D6">
+        <v>290</v>
       </c>
       <c r="E6" t="b">
         <v>0</v>
       </c>
-      <c r="K6" t="s">
+      <c r="F6" t="b">
+        <v>0</v>
+      </c>
+      <c r="L6" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -895,17 +909,20 @@
       <c r="C7" t="s">
         <v>45</v>
       </c>
-      <c r="D7" t="b">
-        <v>0</v>
+      <c r="D7">
+        <v>469</v>
       </c>
       <c r="E7" t="b">
         <v>0</v>
       </c>
-      <c r="K7" t="s">
+      <c r="F7" t="b">
+        <v>0</v>
+      </c>
+      <c r="L7" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>46</v>
       </c>
@@ -915,17 +932,20 @@
       <c r="C8" t="s">
         <v>45</v>
       </c>
-      <c r="D8" t="b">
-        <v>0</v>
+      <c r="D8">
+        <v>330</v>
       </c>
       <c r="E8" t="b">
         <v>0</v>
       </c>
-      <c r="K8" t="s">
+      <c r="F8" t="b">
+        <v>0</v>
+      </c>
+      <c r="L8" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>48</v>
       </c>
@@ -935,17 +955,17 @@
       <c r="C9" t="s">
         <v>50</v>
       </c>
-      <c r="D9" t="b">
-        <v>0</v>
-      </c>
       <c r="E9" t="b">
         <v>0</v>
       </c>
-      <c r="K9" t="s">
+      <c r="F9" t="b">
+        <v>0</v>
+      </c>
+      <c r="L9" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>51</v>
       </c>
@@ -955,17 +975,17 @@
       <c r="C10" t="s">
         <v>42</v>
       </c>
-      <c r="D10" t="b">
-        <v>0</v>
-      </c>
       <c r="E10" t="b">
         <v>0</v>
       </c>
-      <c r="K10" t="s">
+      <c r="F10" t="b">
+        <v>0</v>
+      </c>
+      <c r="L10" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>52</v>
       </c>
@@ -975,17 +995,17 @@
       <c r="C11" t="s">
         <v>53</v>
       </c>
-      <c r="D11" t="b">
-        <v>0</v>
-      </c>
       <c r="E11" t="b">
         <v>0</v>
       </c>
-      <c r="K11" t="s">
+      <c r="F11" t="b">
+        <v>0</v>
+      </c>
+      <c r="L11" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>54</v>
       </c>
@@ -995,17 +1015,17 @@
       <c r="C12" t="s">
         <v>56</v>
       </c>
-      <c r="D12" t="b">
-        <v>0</v>
-      </c>
       <c r="E12" t="b">
         <v>0</v>
       </c>
-      <c r="K12" t="s">
+      <c r="F12" t="b">
+        <v>0</v>
+      </c>
+      <c r="L12" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>57</v>
       </c>
@@ -1015,17 +1035,17 @@
       <c r="C13" t="s">
         <v>59</v>
       </c>
-      <c r="D13" t="b">
+      <c r="E13" t="b">
         <v>1</v>
       </c>
-      <c r="E13" t="b">
-        <v>0</v>
-      </c>
-      <c r="K13" t="s">
+      <c r="F13" t="b">
+        <v>0</v>
+      </c>
+      <c r="L13" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>60</v>
       </c>
@@ -1035,17 +1055,17 @@
       <c r="C14" t="s">
         <v>56</v>
       </c>
-      <c r="D14" t="b">
+      <c r="E14" t="b">
         <v>1</v>
       </c>
-      <c r="E14" t="b">
-        <v>0</v>
-      </c>
-      <c r="K14" t="s">
+      <c r="F14" t="b">
+        <v>0</v>
+      </c>
+      <c r="L14" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>61</v>
       </c>
@@ -1055,17 +1075,17 @@
       <c r="C15" t="s">
         <v>42</v>
       </c>
-      <c r="D15" t="b">
-        <v>0</v>
-      </c>
       <c r="E15" t="b">
         <v>0</v>
       </c>
-      <c r="K15" t="s">
+      <c r="F15" t="b">
+        <v>0</v>
+      </c>
+      <c r="L15" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>63</v>
       </c>
@@ -1075,17 +1095,20 @@
       <c r="C16" t="s">
         <v>45</v>
       </c>
-      <c r="D16" t="b">
-        <v>0</v>
+      <c r="D16">
+        <v>297</v>
       </c>
       <c r="E16" t="b">
         <v>0</v>
       </c>
-      <c r="K16" t="s">
+      <c r="F16" t="b">
+        <v>0</v>
+      </c>
+      <c r="L16" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>65</v>
       </c>
@@ -1095,17 +1118,17 @@
       <c r="C17" t="s">
         <v>42</v>
       </c>
-      <c r="D17" t="b">
-        <v>0</v>
-      </c>
       <c r="E17" t="b">
         <v>0</v>
       </c>
-      <c r="K17" t="s">
+      <c r="F17" t="b">
+        <v>0</v>
+      </c>
+      <c r="L17" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>67</v>
       </c>
@@ -1115,17 +1138,20 @@
       <c r="C18" t="s">
         <v>45</v>
       </c>
-      <c r="D18" t="b">
-        <v>0</v>
+      <c r="D18">
+        <v>414</v>
       </c>
       <c r="E18" t="b">
         <v>0</v>
       </c>
-      <c r="K18" t="s">
+      <c r="F18" t="b">
+        <v>0</v>
+      </c>
+      <c r="L18" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>69</v>
       </c>
@@ -1135,17 +1161,20 @@
       <c r="C19" t="s">
         <v>37</v>
       </c>
-      <c r="D19" t="b">
-        <v>0</v>
+      <c r="D19">
+        <v>270</v>
       </c>
       <c r="E19" t="b">
         <v>0</v>
       </c>
-      <c r="K19" t="s">
+      <c r="F19" t="b">
+        <v>0</v>
+      </c>
+      <c r="L19" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>71</v>
       </c>
@@ -1155,17 +1184,20 @@
       <c r="C20" t="s">
         <v>37</v>
       </c>
-      <c r="D20" t="b">
-        <v>0</v>
+      <c r="D20">
+        <v>296</v>
       </c>
       <c r="E20" t="b">
         <v>0</v>
       </c>
-      <c r="K20" t="s">
+      <c r="F20" t="b">
+        <v>0</v>
+      </c>
+      <c r="L20" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>73</v>
       </c>
@@ -1175,17 +1207,20 @@
       <c r="C21" t="s">
         <v>45</v>
       </c>
-      <c r="D21" t="b">
-        <v>0</v>
+      <c r="D21">
+        <v>353</v>
       </c>
       <c r="E21" t="b">
         <v>0</v>
       </c>
-      <c r="K21" t="s">
+      <c r="F21" t="b">
+        <v>0</v>
+      </c>
+      <c r="L21" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>75</v>
       </c>
@@ -1195,17 +1230,17 @@
       <c r="C22" t="s">
         <v>59</v>
       </c>
-      <c r="D22" t="b">
+      <c r="E22" t="b">
         <v>1</v>
       </c>
-      <c r="E22" t="b">
-        <v>0</v>
-      </c>
-      <c r="K22" t="s">
+      <c r="F22" t="b">
+        <v>0</v>
+      </c>
+      <c r="L22" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>77</v>
       </c>
@@ -1215,17 +1250,17 @@
       <c r="C23" t="s">
         <v>59</v>
       </c>
-      <c r="D23" t="b">
+      <c r="E23" t="b">
         <v>1</v>
       </c>
-      <c r="E23" t="b">
-        <v>0</v>
-      </c>
-      <c r="K23" t="s">
+      <c r="F23" t="b">
+        <v>0</v>
+      </c>
+      <c r="L23" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>79</v>
       </c>
@@ -1235,17 +1270,17 @@
       <c r="C24" t="s">
         <v>59</v>
       </c>
-      <c r="D24" t="b">
+      <c r="E24" t="b">
         <v>1</v>
       </c>
-      <c r="E24" t="b">
-        <v>0</v>
-      </c>
-      <c r="K24" t="s">
+      <c r="F24" t="b">
+        <v>0</v>
+      </c>
+      <c r="L24" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>81</v>
       </c>
@@ -1255,17 +1290,17 @@
       <c r="C25" t="s">
         <v>59</v>
       </c>
-      <c r="D25" t="b">
+      <c r="E25" t="b">
         <v>1</v>
       </c>
-      <c r="E25" t="b">
-        <v>0</v>
-      </c>
-      <c r="K25" t="s">
+      <c r="F25" t="b">
+        <v>0</v>
+      </c>
+      <c r="L25" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>83</v>
       </c>
@@ -1275,17 +1310,17 @@
       <c r="C26" t="s">
         <v>45</v>
       </c>
-      <c r="D26" t="b">
-        <v>0</v>
-      </c>
       <c r="E26" t="b">
         <v>0</v>
       </c>
-      <c r="K26" t="s">
+      <c r="F26" t="b">
+        <v>0</v>
+      </c>
+      <c r="L26" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>85</v>
       </c>
@@ -1295,17 +1330,20 @@
       <c r="C27" t="s">
         <v>56</v>
       </c>
-      <c r="D27" t="b">
-        <v>0</v>
+      <c r="D27">
+        <v>202</v>
       </c>
       <c r="E27" t="b">
         <v>0</v>
       </c>
-      <c r="K27" t="s">
+      <c r="F27" t="b">
+        <v>0</v>
+      </c>
+      <c r="L27" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>87</v>
       </c>
@@ -1315,17 +1353,17 @@
       <c r="C28" t="s">
         <v>50</v>
       </c>
-      <c r="D28" t="b">
-        <v>0</v>
-      </c>
       <c r="E28" t="b">
         <v>0</v>
       </c>
-      <c r="K28" t="s">
+      <c r="F28" t="b">
+        <v>0</v>
+      </c>
+      <c r="L28" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>89</v>
       </c>
@@ -1335,17 +1373,17 @@
       <c r="C29" t="s">
         <v>50</v>
       </c>
-      <c r="D29" t="b">
-        <v>0</v>
-      </c>
       <c r="E29" t="b">
         <v>0</v>
       </c>
-      <c r="K29" t="s">
+      <c r="F29" t="b">
+        <v>0</v>
+      </c>
+      <c r="L29" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>91</v>
       </c>
@@ -1355,17 +1393,17 @@
       <c r="C30" t="s">
         <v>53</v>
       </c>
-      <c r="D30" t="b">
-        <v>0</v>
-      </c>
       <c r="E30" t="b">
         <v>0</v>
       </c>
-      <c r="K30" t="s">
+      <c r="F30" t="b">
+        <v>0</v>
+      </c>
+      <c r="L30" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>92</v>
       </c>
@@ -1375,17 +1413,17 @@
       <c r="C31" t="s">
         <v>56</v>
       </c>
-      <c r="D31" t="b">
+      <c r="E31" t="b">
         <v>1</v>
       </c>
-      <c r="E31" t="b">
-        <v>0</v>
-      </c>
-      <c r="K31" t="s">
+      <c r="F31" t="b">
+        <v>0</v>
+      </c>
+      <c r="L31" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>94</v>
       </c>
@@ -1395,17 +1433,20 @@
       <c r="C32" t="s">
         <v>37</v>
       </c>
-      <c r="D32" t="b">
-        <v>0</v>
+      <c r="D32">
+        <v>334</v>
       </c>
       <c r="E32" t="b">
         <v>0</v>
       </c>
-      <c r="K32" t="s">
+      <c r="F32" t="b">
+        <v>0</v>
+      </c>
+      <c r="L32" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>96</v>
       </c>
@@ -1415,17 +1456,17 @@
       <c r="C33" t="s">
         <v>42</v>
       </c>
-      <c r="D33" t="b">
-        <v>0</v>
-      </c>
       <c r="E33" t="b">
         <v>0</v>
       </c>
-      <c r="K33" t="s">
+      <c r="F33" t="b">
+        <v>0</v>
+      </c>
+      <c r="L33" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>98</v>
       </c>
@@ -1435,13 +1476,13 @@
       <c r="C34" t="s">
         <v>45</v>
       </c>
-      <c r="D34" t="b">
-        <v>0</v>
-      </c>
       <c r="E34" t="b">
         <v>0</v>
       </c>
-      <c r="K34" t="s">
+      <c r="F34" t="b">
+        <v>0</v>
+      </c>
+      <c r="L34" t="s">
         <v>99</v>
       </c>
     </row>

</xml_diff>